<commit_message>
added search Banner API'S
</commit_message>
<xml_diff>
--- a/TestData/Catalog/Banner_Api.xlsx
+++ b/TestData/Catalog/Banner_Api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.gl\Desktop\onmobile\TestData\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F3DDB8-3B89-452B-BA91-694830C9BDA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A227DF5-D21C-464E-8DEC-550326CDAA48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="10" activeTab="11" xr2:uid="{9198B136-2ACC-4A81-8A9E-1453B697301F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="16" xr2:uid="{9198B136-2ACC-4A81-8A9E-1453B697301F}"/>
   </bookViews>
   <sheets>
     <sheet name="CREATE_BANNER_POSITIVE_SHEET" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,12 @@
     <sheet name="DELETE_BANNER_COLLECTION_POSITI" sheetId="10" r:id="rId10"/>
     <sheet name="GET_BANNER_COLLECTION_BY_ID_POS" sheetId="11" r:id="rId11"/>
     <sheet name="GET_BANNER_COLLECTION_BY_ID_NEG" sheetId="12" r:id="rId12"/>
+    <sheet name="GET_ALL_BANNER_COLLECTION_POSIT" sheetId="13" r:id="rId13"/>
+    <sheet name="SEARCH_BANNER_COLLECTION_POSITI" sheetId="15" r:id="rId14"/>
+    <sheet name="SEARCH_BANNER_BY_NAME_POSITIVE_" sheetId="17" r:id="rId15"/>
+    <sheet name="GET_ALL_BANNER_COLLECTION_NEGAT" sheetId="14" r:id="rId16"/>
+    <sheet name="SEARCH_BANNER_BY_NAME_NEGATIVE_" sheetId="18" r:id="rId17"/>
+    <sheet name="SEARCH_BANNER_COLLECTION_NEGATI" sheetId="16" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="79">
   <si>
     <t>Test case</t>
   </si>
@@ -228,6 +234,51 @@
   </si>
   <si>
     <t>NAVEEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get All Banner Collection with valid data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get All Banner Collection with Invalid store ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get All Banner Collection with Invalid query Param i.e response </t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Search Banner Collection By Name with valid Test Data</t>
+  </si>
+  <si>
+    <t>searchItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search By Banner Collection by name with Invalid store id </t>
+  </si>
+  <si>
+    <t>Search By Banner Collection by name with Invalid blank Search Iteam</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Search Banner By Name with Valid Test Data</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Search Banner By Name with inValid Store ID</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>Search Banner By Name with inValid Search Iteam</t>
+  </si>
+  <si>
+    <t>Search Banner By Name with  blank  Search Iteam</t>
   </si>
 </sst>
 </file>
@@ -786,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A236F48C-6BB9-48E4-97F3-121C6A937397}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +920,345 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4260125-3232-4C09-ABCB-B6914235BD44}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>168</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F1C066-3CF0-425E-AB34-44AE86BE6495}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC28FD52-2C90-4054-BFD8-BDE6D9EB512B}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45043FA-4268-4AC4-B685-981EAAFDA9C4}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>404</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>404</v>
+      </c>
+      <c r="C3">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73E1F56-A38C-4109-99C6-E0B607D89A3F}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>404</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680CAE4B-AF50-4963-9566-961B75FEC0A0}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>404</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>